<commit_message>
update code from duongdx
</commit_message>
<xml_diff>
--- a/src/aspnet-core 7.0/src/KNTC.HttpApi.Host/wwwroot/ExcelTemplate/Complain.xlsx
+++ b/src/aspnet-core 7.0/src/KNTC.HttpApi.Host/wwwroot/ExcelTemplate/Complain.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Duong\Projects\Hau\KNTC\Code\PostgreSQL\src\server\src\KNTC.HttpApi.Host\wwwroot\ExcelTemplate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Duong\Projects\Hau\KNTC\Code\PostgreSQL\src\aspnet-core 7.0\src\KNTC.HttpApi.Host\wwwroot\ExcelTemplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,9 +15,9 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$17:$O$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$17:$P$17</definedName>
   </definedNames>
-  <calcPr calcId="162913" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>HTTTTT Quản lý Đơn thư Khiếu nại, Tố cáo</t>
   </si>
@@ -137,6 +137,9 @@
   </si>
   <si>
     <t>Thẩm quyền GQKN lần II</t>
+  </si>
+  <si>
+    <t>Trạng thái</t>
   </si>
 </sst>
 </file>
@@ -576,10 +579,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O26"/>
+  <dimension ref="A1:P26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:O4"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -587,65 +590,67 @@
     <col min="1" max="1" width="5.109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="10.6640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="15.109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="14" style="1" customWidth="1"/>
-    <col min="6" max="6" width="25.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.21875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="20.5546875" style="1" customWidth="1"/>
     <col min="7" max="7" width="16.44140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="17.5546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="15.6640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="14.77734375" style="1" customWidth="1"/>
-    <col min="11" max="12" width="14.6640625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="13.77734375" style="1" customWidth="1"/>
-    <col min="14" max="14" width="14.6640625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="18" style="1" customWidth="1"/>
-    <col min="16" max="16384" width="8.88671875" style="1"/>
+    <col min="8" max="8" width="12" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14.44140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="15.6640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5546875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="14.109375" style="1" customWidth="1"/>
+    <col min="13" max="13" width="12.21875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="11.33203125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="13.6640625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="13.33203125" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
         <v>23</v>
       </c>
       <c r="B1" s="14"/>
       <c r="C1" s="14"/>
       <c r="D1" s="14"/>
-      <c r="H1" s="11"/>
       <c r="I1" s="11"/>
-      <c r="J1" s="15" t="s">
+      <c r="J1" s="11"/>
+      <c r="K1" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="K1" s="15"/>
       <c r="L1" s="15"/>
       <c r="M1" s="15"/>
-      <c r="N1" s="11"/>
-    </row>
-    <row r="2" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="N1" s="15"/>
+      <c r="O1" s="11"/>
+    </row>
+    <row r="2" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
         <v>25</v>
       </c>
       <c r="B2" s="14"/>
       <c r="C2" s="14"/>
       <c r="D2" s="14"/>
-      <c r="H2" s="11"/>
       <c r="I2" s="11"/>
-      <c r="J2" s="15" t="s">
+      <c r="J2" s="11"/>
+      <c r="K2" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="K2" s="15"/>
       <c r="L2" s="15"/>
       <c r="M2" s="15"/>
-      <c r="N2" s="11"/>
-    </row>
-    <row r="3" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="H3" s="12"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="11"/>
+    </row>
+    <row r="3" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="I3" s="12"/>
-      <c r="J3" s="16" t="s">
+      <c r="J3" s="12"/>
+      <c r="K3" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="K3" s="16"/>
       <c r="L3" s="16"/>
       <c r="M3" s="16"/>
-    </row>
-    <row r="4" spans="1:15" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="N3" s="16"/>
+    </row>
+    <row r="4" spans="1:16" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A4" s="13" t="s">
         <v>30</v>
       </c>
@@ -663,66 +668,67 @@
       <c r="M4" s="13"/>
       <c r="N4" s="13"/>
       <c r="O4" s="13"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P4" s="13"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B5" s="3"/>
       <c r="D5" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B6" s="3"/>
       <c r="D6" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D7" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E8" s="6"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D9" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E9" s="6"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D10" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E10" s="6"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D11" s="2" t="s">
         <v>21</v>
       </c>
       <c r="E11" s="6"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D12" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E12" s="6"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D13" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E13" s="6"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D14" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:15" s="10" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" s="10" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
         <v>1</v>
       </c>
@@ -745,31 +751,34 @@
         <v>4</v>
       </c>
       <c r="H16" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="I16" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="I16" s="9" t="s">
+      <c r="J16" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="J16" s="9" t="s">
+      <c r="K16" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="K16" s="9" t="s">
+      <c r="L16" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="L16" s="9" t="s">
+      <c r="M16" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="M16" s="9" t="s">
+      <c r="N16" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="N16" s="9" t="s">
+      <c r="O16" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="O16" s="9" t="s">
+      <c r="P16" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:15" s="10" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" s="10" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="9">
         <v>1</v>
       </c>
@@ -815,8 +824,11 @@
       <c r="O17" s="9">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P17" s="9">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>1</v>
       </c>
@@ -828,40 +840,41 @@
       <c r="G18" s="7">
         <v>44567.625</v>
       </c>
-      <c r="H18" s="5"/>
-      <c r="I18" s="7">
+      <c r="H18" s="7"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="7">
         <v>44567.625</v>
       </c>
-      <c r="J18" s="8">
+      <c r="K18" s="8">
         <v>44567.375</v>
       </c>
-      <c r="K18" s="5"/>
       <c r="L18" s="5"/>
-      <c r="M18" s="8">
+      <c r="M18" s="5"/>
+      <c r="N18" s="8">
         <v>44567.375</v>
       </c>
-      <c r="N18" s="5"/>
       <c r="O18" s="5"/>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J22" s="2" t="s">
+      <c r="P18" s="5"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K22" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A17:O17"/>
+  <autoFilter ref="A17:P17"/>
   <mergeCells count="6">
-    <mergeCell ref="A4:O4"/>
+    <mergeCell ref="A4:P4"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:D2"/>
-    <mergeCell ref="J1:M1"/>
-    <mergeCell ref="J2:M2"/>
-    <mergeCell ref="J3:M3"/>
+    <mergeCell ref="K1:N1"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="K3:N3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Sửa các tiêu đề Tỉnh/TP -> Tỉnh, Quận/Huyện -> Huyện/TP trong form, view và report
</commit_message>
<xml_diff>
--- a/src/aspnet-core 7.0/src/KNTC.HttpApi.Host/wwwroot/ExcelTemplate/Complain.xlsx
+++ b/src/aspnet-core 7.0/src/KNTC.HttpApi.Host/wwwroot/ExcelTemplate/Complain.xlsx
@@ -67,15 +67,6 @@
     <t>Kết quả GQKN lần I</t>
   </si>
   <si>
-    <t>Quận/Huyện:</t>
-  </si>
-  <si>
-    <t>Tỉnh/TP:</t>
-  </si>
-  <si>
-    <t>Xã/Phường:</t>
-  </si>
-  <si>
     <t>Kết quả:</t>
   </si>
   <si>
@@ -140,6 +131,15 @@
   </si>
   <si>
     <t>Trạng thái</t>
+  </si>
+  <si>
+    <t>Huyện/TP:</t>
+  </si>
+  <si>
+    <t>Tỉnh:</t>
+  </si>
+  <si>
+    <t>Phường/Xã:</t>
   </si>
 </sst>
 </file>
@@ -582,7 +582,7 @@
   <dimension ref="A1:P26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="D8" sqref="D8:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -608,7 +608,7 @@
   <sheetData>
     <row r="1" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B1" s="14"/>
       <c r="C1" s="14"/>
@@ -616,7 +616,7 @@
       <c r="I1" s="11"/>
       <c r="J1" s="11"/>
       <c r="K1" s="15" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="L1" s="15"/>
       <c r="M1" s="15"/>
@@ -625,7 +625,7 @@
     </row>
     <row r="2" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B2" s="14"/>
       <c r="C2" s="14"/>
@@ -633,7 +633,7 @@
       <c r="I2" s="11"/>
       <c r="J2" s="11"/>
       <c r="K2" s="15" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="L2" s="15"/>
       <c r="M2" s="15"/>
@@ -644,7 +644,7 @@
       <c r="I3" s="12"/>
       <c r="J3" s="12"/>
       <c r="K3" s="16" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="L3" s="16"/>
       <c r="M3" s="16"/>
@@ -652,7 +652,7 @@
     </row>
     <row r="4" spans="1:16" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A4" s="13" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B4" s="13"/>
       <c r="C4" s="13"/>
@@ -673,59 +673,59 @@
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B5" s="3"/>
       <c r="D5" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B6" s="3"/>
       <c r="D6" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D7" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D8" s="2" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="E8" s="6"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D9" s="2" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="E9" s="6"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D10" s="2" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="E10" s="6"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D11" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E11" s="6"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D12" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E12" s="6"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D13" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E13" s="6"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D14" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="10" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -733,13 +733,13 @@
         <v>1</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E16" s="9" t="s">
         <v>2</v>
@@ -751,7 +751,7 @@
         <v>4</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="I16" s="9" t="s">
         <v>5</v>
@@ -763,19 +763,19 @@
         <v>7</v>
       </c>
       <c r="L16" s="9" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="M16" s="9" t="s">
         <v>8</v>
       </c>
       <c r="N16" s="9" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="O16" s="9" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="P16" s="9" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="10" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -858,7 +858,7 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="K22" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">

</xml_diff>